<commit_message>
version 5.2 as described in the Roadmap (Projects)
</commit_message>
<xml_diff>
--- a/Ministers.xlsx
+++ b/Ministers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KCvan\Dropbox\Jupyter Lab\De Vijfde Macht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruiker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBA7D24-4375-44A6-A527-5EF2D6CD4EC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8060794F-CB98-45E9-B81B-B0D5928D33FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -179,13 +179,127 @@
   </si>
   <si>
     <t>Staatssecretaris van Volksgezondheid, Welzijn en Sport</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>Cabinet</t>
+  </si>
+  <si>
+    <t>Rutte_3</t>
+  </si>
+  <si>
+    <t>Zijlstra, Halbe</t>
+  </si>
+  <si>
+    <t>Snel, Menno</t>
+  </si>
+  <si>
+    <t>Harbers, Mark</t>
+  </si>
+  <si>
+    <t>Rutte_2</t>
+  </si>
+  <si>
+    <t>Asscher, Lodewijk</t>
+  </si>
+  <si>
+    <t>Plasterk, Ronald</t>
+  </si>
+  <si>
+    <t>Timmermans, Frans</t>
+  </si>
+  <si>
+    <t>Koenders, Bert</t>
+  </si>
+  <si>
+    <t>Dijsselbloem, Jeroen</t>
+  </si>
+  <si>
+    <t>Opstelten, Ivo</t>
+  </si>
+  <si>
+    <t>Minister van Veiligheid en Justitie</t>
+  </si>
+  <si>
+    <t>Steur van der, Ard</t>
+  </si>
+  <si>
+    <t>Kamp, Henk</t>
+  </si>
+  <si>
+    <t>Minister van Economische Zaken</t>
+  </si>
+  <si>
+    <t>Hennis-Plasschaert, Jeanine</t>
+  </si>
+  <si>
+    <t>Dijkhoff, Klaas</t>
+  </si>
+  <si>
+    <t>Schippers, Edith</t>
+  </si>
+  <si>
+    <t>Bussemaker, Jet</t>
+  </si>
+  <si>
+    <t>Schultz van Haegen, Melanie</t>
+  </si>
+  <si>
+    <t>Minister van Infrastructuur en Milieu</t>
+  </si>
+  <si>
+    <t>Minister van Wonen en Rijkdienst</t>
+  </si>
+  <si>
+    <t>Ploumen, Lilianne</t>
+  </si>
+  <si>
+    <t>Minister van Buitenlandse Handel en Ontwikkelingssamenwerking</t>
+  </si>
+  <si>
+    <t>Weekers, Frans</t>
+  </si>
+  <si>
+    <t>Teeven, Fred</t>
+  </si>
+  <si>
+    <t>Staatssecretaris van Veiligheid en Justitie</t>
+  </si>
+  <si>
+    <t>Verdaas, Co</t>
+  </si>
+  <si>
+    <t>Staatssecretaris van Economische Zaken</t>
+  </si>
+  <si>
+    <t>Dijksma, Sharon</t>
+  </si>
+  <si>
+    <t>Dam van, Martijn</t>
+  </si>
+  <si>
+    <t>Klijnsma, Jetta</t>
+  </si>
+  <si>
+    <t>Staatssecretaris van Onderwijs, Cultuur en Wetenschap</t>
+  </si>
+  <si>
+    <t>Mansveld, Wilma</t>
+  </si>
+  <si>
+    <t>Staatssecretaris van Infrastructuur en Milieu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,7 +310,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,11 +363,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -541,243 +672,1100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="69.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43770</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43935</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43144</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43166</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C10" s="1">
+        <v>43166</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C11" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C12" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C13" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C14" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C15" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C16" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C17" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C18" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C19" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D19" s="1">
+        <v>43909</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C20" s="1">
+        <v>43913</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C21" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C22" s="1">
+        <v>43770</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43935</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C23" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43770</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43935</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C25" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C26" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43817</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B28" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C28" s="1">
+        <v>43859</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C29" s="1">
+        <v>43859</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C30" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D30" s="1">
+        <v>43770</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43935</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43034</v>
+      </c>
+      <c r="D32" s="1">
+        <v>43606</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C33" s="1">
+        <v>43627</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B34" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C34" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" t="s">
         <v>52</v>
       </c>
+      <c r="C35" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D37" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D38" s="1">
+        <v>42550</v>
+      </c>
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42550</v>
+      </c>
+      <c r="D39" s="1">
+        <v>42629</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42629</v>
+      </c>
+      <c r="D40" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D41" s="1">
+        <v>41929</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="1">
+        <v>41929</v>
+      </c>
+      <c r="D42" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D43" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D44" s="1">
+        <v>42073</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="1">
+        <v>42073</v>
+      </c>
+      <c r="D45" s="1">
+        <v>42083</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="1">
+        <v>42083</v>
+      </c>
+      <c r="D46" s="1">
+        <v>42762</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="1">
+        <v>42762</v>
+      </c>
+      <c r="D47" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D48" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D49" s="1">
+        <v>43012</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1">
+        <v>43012</v>
+      </c>
+      <c r="D50" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D51" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D52" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D53" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D54" s="1">
+        <v>42762</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D55" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D56" s="1">
+        <v>41669</v>
+      </c>
+      <c r="E56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="1">
+        <v>41674</v>
+      </c>
+      <c r="D57" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D58" s="1">
+        <v>42073</v>
+      </c>
+      <c r="E58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="1">
+        <v>42073</v>
+      </c>
+      <c r="D59" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D60" s="1">
+        <v>41249</v>
+      </c>
+      <c r="E60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="1">
+        <v>41261</v>
+      </c>
+      <c r="D61" s="1">
+        <v>42313</v>
+      </c>
+      <c r="E61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="1">
+        <v>42311</v>
+      </c>
+      <c r="D62" s="1">
+        <v>42979</v>
+      </c>
+      <c r="E62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D63" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D64" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D65" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C66" s="1">
+        <v>41218</v>
+      </c>
+      <c r="D66" s="1">
+        <v>42305</v>
+      </c>
+      <c r="E66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="1">
+        <v>42313</v>
+      </c>
+      <c r="D67" s="1">
+        <v>43034</v>
+      </c>
+      <c r="E67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>